<commit_message>
Finished find suggestions and add start/end dates
</commit_message>
<xml_diff>
--- a/codeToDo.xlsx
+++ b/codeToDo.xlsx
@@ -977,7 +977,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:B28"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1007,7 +1007,7 @@
         <f>A2+1</f>
         <v>3</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1016,7 +1016,7 @@
         <f t="shared" ref="A4:A16" si="0">A3+1</f>
         <v>4</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="3" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1025,7 +1025,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1043,7 +1043,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1061,7 +1061,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1070,7 +1070,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="3" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1129,17 +1129,17 @@
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="3" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated to-do and name change to generate itinerary
</commit_message>
<xml_diff>
--- a/codeToDo.xlsx
+++ b/codeToDo.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CanadianRunna\Desktop\Website\plannedJourneysGit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ian MacIsaac\Desktop\Website\plannedJourneysGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27876" windowHeight="13020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="13020" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Updated-Todo" sheetId="2" r:id="rId2"/>
+    <sheet name="Update to-do 08-19-2018" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="67">
   <si>
     <t>Code</t>
   </si>
@@ -187,6 +188,45 @@
   </si>
   <si>
     <t>Dates First</t>
+  </si>
+  <si>
+    <t>Think about new title on Plan a Trip Page</t>
+  </si>
+  <si>
+    <t>Think about splitting up locations and activities</t>
+  </si>
+  <si>
+    <t>Pull times from locations in order to correctly generate itinerary based on when they're open</t>
+  </si>
+  <si>
+    <t>Dynamic clicking on itinerary</t>
+  </si>
+  <si>
+    <t>Web spiders to parse information for top search locations to put into database for faster loading</t>
+  </si>
+  <si>
+    <t>Data analytics for pulling information</t>
+  </si>
+  <si>
+    <t>Database of items necessary based on activities in your trip</t>
+  </si>
+  <si>
+    <t>Generate itinerary creates a new page where the plan is full page with a map on the bottom with all of the directions from place to place where you can click on legs on either the map or the itinerary to highlight them, see the travel time, change mode of transportation, etc.</t>
+  </si>
+  <si>
+    <t>Create database that is capable  of saving user names / passwords</t>
+  </si>
+  <si>
+    <t>Create database for itineraries</t>
+  </si>
+  <si>
+    <t>Back end to calculate the itinerary</t>
+  </si>
+  <si>
+    <t>Clickable google maps directions based on the calculated itinerary page</t>
+  </si>
+  <si>
+    <t>Create Back End (Stores Username / Password, Calculates Itinerary, Stores Itinerary, Shows Itinerary, Parses Data &amp; Grabs data from internet etc.)</t>
   </si>
 </sst>
 </file>
@@ -553,18 +593,18 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="148.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="148.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -581,7 +621,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -598,7 +638,7 @@
         <v>43218</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f>A2+1</f>
         <v>2</v>
@@ -616,7 +656,7 @@
         <v>43218</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <f t="shared" ref="A4:A24" si="0">A3+1</f>
         <v>3</v>
@@ -634,7 +674,7 @@
         <v>43219</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -647,7 +687,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -661,7 +701,7 @@
       <c r="D6" s="3"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -675,7 +715,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -688,7 +728,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -702,7 +742,7 @@
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -723,7 +763,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -744,7 +784,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -762,7 +802,7 @@
         <v>43219</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -780,7 +820,7 @@
         <v>43219</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -798,7 +838,7 @@
         <v>43219</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -816,7 +856,7 @@
         <v>43221</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -834,7 +874,7 @@
         <v>43221</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -847,7 +887,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -860,7 +900,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -873,7 +913,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -886,7 +926,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -904,7 +944,7 @@
         <v>43223</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -922,7 +962,7 @@
         <v>43225</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -940,7 +980,7 @@
         <v>43225</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -955,7 +995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
@@ -976,16 +1016,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="91.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -993,7 +1033,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <f>A1+1</f>
         <v>2</v>
@@ -1002,7 +1042,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>3</v>
@@ -1011,7 +1051,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A16" si="0">A3+1</f>
         <v>4</v>
@@ -1020,7 +1060,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1029,7 +1069,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1038,7 +1078,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1047,7 +1087,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1056,7 +1096,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1065,7 +1105,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1074,7 +1114,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1083,7 +1123,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1092,7 +1132,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1101,7 +1141,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1110,7 +1150,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1119,7 +1159,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1128,29 +1168,115 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CSS for Main Search
</commit_message>
<xml_diff>
--- a/codeToDo.xlsx
+++ b/codeToDo.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CanadianRunna\Desktop\Website\plannedJourneysGit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ian MacIsaac\Desktop\Website\plannedJourneysGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27876" windowHeight="13020" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="13020" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -687,15 +687,15 @@
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="148.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="148.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -712,7 +712,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -729,7 +729,7 @@
         <v>43218</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f>A2+1</f>
         <v>2</v>
@@ -747,7 +747,7 @@
         <v>43218</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <f t="shared" ref="A4:A24" si="0">A3+1</f>
         <v>3</v>
@@ -765,7 +765,7 @@
         <v>43219</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -778,7 +778,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -792,7 +792,7 @@
       <c r="D6" s="3"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -806,7 +806,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -819,7 +819,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -833,7 +833,7 @@
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -854,7 +854,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -875,7 +875,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -893,7 +893,7 @@
         <v>43219</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -911,7 +911,7 @@
         <v>43219</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -929,7 +929,7 @@
         <v>43219</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -947,7 +947,7 @@
         <v>43221</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -965,7 +965,7 @@
         <v>43221</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -978,7 +978,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -991,7 +991,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1004,7 +1004,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1035,7 +1035,7 @@
         <v>43223</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1053,7 +1053,7 @@
         <v>43225</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1071,7 +1071,7 @@
         <v>43225</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1086,7 +1086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
@@ -1111,12 +1111,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="91.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <f>A1+1</f>
         <v>2</v>
@@ -1133,7 +1133,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>3</v>
@@ -1142,7 +1142,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A16" si="0">A3+1</f>
         <v>4</v>
@@ -1151,7 +1151,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1160,7 +1160,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1169,7 +1169,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1178,7 +1178,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1187,7 +1187,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1196,7 +1196,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1205,7 +1205,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1214,7 +1214,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1223,7 +1223,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1232,7 +1232,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1241,7 +1241,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1250,7 +1250,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1259,27 +1259,27 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>50</v>
       </c>
@@ -1298,9 +1298,9 @@
       <selection activeCell="A35" sqref="A35:A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>A1+1</f>
         <v>2</v>
@@ -1317,7 +1317,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A34" si="0">A2+1</f>
         <v>3</v>
@@ -1326,7 +1326,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1335,7 +1335,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1344,7 +1344,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1353,7 +1353,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1362,7 +1362,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1371,7 +1371,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1380,7 +1380,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1389,7 +1389,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1398,7 +1398,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1407,7 +1407,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1416,7 +1416,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1425,7 +1425,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1434,7 +1434,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>A15+1</f>
         <v>16</v>
@@ -1443,7 +1443,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1452,7 +1452,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1461,7 +1461,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1470,7 +1470,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1479,7 +1479,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1488,7 +1488,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1497,7 +1497,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1506,7 +1506,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1515,7 +1515,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1524,7 +1524,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1533,7 +1533,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1542,7 +1542,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1551,7 +1551,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1560,7 +1560,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1569,7 +1569,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1578,7 +1578,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1587,7 +1587,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1596,7 +1596,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1613,32 +1613,35 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="64" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>A1+1</f>
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A15" si="0">A2+1</f>
         <v>3</v>
@@ -1647,7 +1650,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1656,7 +1659,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1665,7 +1668,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1674,7 +1677,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1683,7 +1686,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1692,7 +1695,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1701,7 +1704,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1710,37 +1713,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaning / Trips Pre-login & Contact Us
</commit_message>
<xml_diff>
--- a/codeToDo.xlsx
+++ b/codeToDo.xlsx
@@ -320,10 +320,10 @@
     <t>Set up database for main page and for Plan a Trip page</t>
   </si>
   <si>
-    <t>Look through other tab for things to do AND START DOING DATABASE</t>
-  </si>
-  <si>
     <t>(Fix resizing for cards, add in email newsletter sign up, add in a final set of 3 cards for Destinations)</t>
+  </si>
+  <si>
+    <t>Look through other tab for things to do AND START DOING DATABASE / PLAN A TRIP PAGE</t>
   </si>
 </sst>
 </file>
@@ -1622,7 +1622,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1665,7 +1665,7 @@
         <v>88</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1682,7 +1682,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1691,7 +1691,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1727,7 +1727,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>